<commit_message>
Updated all files, added in db directory with data dumped file
</commit_message>
<xml_diff>
--- a/pop/summary_deficit.xlsx
+++ b/pop/summary_deficit.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26929"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27022"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16880"/>
@@ -10,6 +10,9 @@
     <sheet name="summary_deficit.csv" sheetId="1" r:id="rId1"/>
     <sheet name="grants" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">summary_deficit.csv!$A$1:$K$129</definedName>
+  </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -23,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="47">
   <si>
     <t>Omaheke and Otjozondjupa Cattle Ranching</t>
   </si>
@@ -161,6 +164,9 @@
   </si>
   <si>
     <t xml:space="preserve">Erongo-Kunene Small Stock and Natural Resources </t>
+  </si>
+  <si>
+    <t>s_def_cash</t>
   </si>
 </sst>
 </file>
@@ -661,11 +667,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J129"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:K129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A70" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J70" sqref="J70"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7:E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -683,7 +690,7 @@
     <col min="11" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1">
+    <row r="1" spans="1:11">
       <c r="A1" s="4" t="s">
         <v>41</v>
       </c>
@@ -714,8 +721,11 @@
       <c r="J1" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" s="4" customFormat="1">
+      <c r="K1" s="4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" hidden="1">
       <c r="A2" s="4" t="s">
         <v>42</v>
       </c>
@@ -748,7 +758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="4" customFormat="1">
+    <row r="3" spans="1:11" hidden="1">
       <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
@@ -781,7 +791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="4" customFormat="1">
+    <row r="4" spans="1:11" hidden="1">
       <c r="A4" s="4" t="s">
         <v>42</v>
       </c>
@@ -814,7 +824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="4" customFormat="1">
+    <row r="5" spans="1:11" hidden="1">
       <c r="A5" s="4" t="s">
         <v>42</v>
       </c>
@@ -847,7 +857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" s="4" customFormat="1">
+    <row r="6" spans="1:11" hidden="1">
       <c r="A6" s="4" t="s">
         <v>42</v>
       </c>
@@ -880,7 +890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="4" customFormat="1">
+    <row r="7" spans="1:11">
       <c r="A7" s="4" t="s">
         <v>42</v>
       </c>
@@ -913,7 +923,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:10" s="4" customFormat="1">
+    <row r="8" spans="1:11" hidden="1">
       <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
@@ -946,7 +956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="4" customFormat="1">
+    <row r="9" spans="1:11" hidden="1">
       <c r="A9" s="4" t="s">
         <v>42</v>
       </c>
@@ -979,7 +989,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" s="4" customFormat="1">
+    <row r="10" spans="1:11" hidden="1">
       <c r="A10" s="4" t="s">
         <v>42</v>
       </c>
@@ -1012,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:10" s="4" customFormat="1">
+    <row r="11" spans="1:11" hidden="1">
       <c r="A11" s="4" t="s">
         <v>42</v>
       </c>
@@ -1045,7 +1055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="4" customFormat="1">
+    <row r="12" spans="1:11" hidden="1">
       <c r="A12" s="4" t="s">
         <v>42</v>
       </c>
@@ -1078,7 +1088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="4" customFormat="1">
+    <row r="13" spans="1:11">
       <c r="A13" s="4" t="s">
         <v>42</v>
       </c>
@@ -1111,7 +1121,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="4" customFormat="1">
+    <row r="14" spans="1:11" hidden="1">
       <c r="A14" s="4" t="s">
         <v>42</v>
       </c>
@@ -1144,7 +1154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="4" customFormat="1">
+    <row r="15" spans="1:11" hidden="1">
       <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
@@ -1177,7 +1187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="4" customFormat="1">
+    <row r="16" spans="1:11" hidden="1">
       <c r="A16" s="4" t="s">
         <v>42</v>
       </c>
@@ -1210,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="4" customFormat="1">
+    <row r="17" spans="1:10" hidden="1">
       <c r="A17" s="4" t="s">
         <v>42</v>
       </c>
@@ -1243,7 +1253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" s="4" customFormat="1">
+    <row r="18" spans="1:10" hidden="1">
       <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
@@ -1276,7 +1286,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" s="4" customFormat="1">
+    <row r="19" spans="1:10" hidden="1">
       <c r="A19" s="4" t="s">
         <v>42</v>
       </c>
@@ -1309,7 +1319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="4" customFormat="1">
+    <row r="20" spans="1:10">
       <c r="A20" s="4" t="s">
         <v>42</v>
       </c>
@@ -1342,7 +1352,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="21" spans="1:10" s="4" customFormat="1">
+    <row r="21" spans="1:10">
       <c r="A21" s="4" t="s">
         <v>42</v>
       </c>
@@ -1375,7 +1385,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="4" customFormat="1">
+    <row r="22" spans="1:10" hidden="1">
       <c r="A22" s="4" t="s">
         <v>42</v>
       </c>
@@ -1408,7 +1418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" s="4" customFormat="1">
+    <row r="23" spans="1:10" hidden="1">
       <c r="A23" s="4" t="s">
         <v>42</v>
       </c>
@@ -1441,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" s="4" customFormat="1">
+    <row r="24" spans="1:10" hidden="1">
       <c r="A24" s="4" t="s">
         <v>42</v>
       </c>
@@ -1474,7 +1484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="4" customFormat="1">
+    <row r="25" spans="1:10" hidden="1">
       <c r="A25" s="4" t="s">
         <v>42</v>
       </c>
@@ -1507,7 +1517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:10" s="4" customFormat="1">
+    <row r="26" spans="1:10" hidden="1">
       <c r="A26" s="4" t="s">
         <v>42</v>
       </c>
@@ -1540,7 +1550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:10" s="4" customFormat="1">
+    <row r="27" spans="1:10" hidden="1">
       <c r="A27" s="4" t="s">
         <v>42</v>
       </c>
@@ -1573,7 +1583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="4" customFormat="1">
+    <row r="28" spans="1:10" hidden="1">
       <c r="A28" s="4" t="s">
         <v>42</v>
       </c>
@@ -1606,7 +1616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" s="4" customFormat="1">
+    <row r="29" spans="1:10">
       <c r="A29" s="4" t="s">
         <v>42</v>
       </c>
@@ -1639,7 +1649,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="4" customFormat="1">
+    <row r="30" spans="1:10" hidden="1">
       <c r="A30" s="4" t="s">
         <v>42</v>
       </c>
@@ -1672,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" s="4" customFormat="1">
+    <row r="31" spans="1:10" hidden="1">
       <c r="A31" s="4" t="s">
         <v>42</v>
       </c>
@@ -1705,7 +1715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" s="4" customFormat="1">
+    <row r="32" spans="1:10" hidden="1">
       <c r="A32" s="4" t="s">
         <v>42</v>
       </c>
@@ -1738,7 +1748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:10" s="4" customFormat="1">
+    <row r="33" spans="1:10" hidden="1">
       <c r="A33" s="4" t="s">
         <v>42</v>
       </c>
@@ -1771,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="4" customFormat="1">
+    <row r="34" spans="1:10" hidden="1">
       <c r="A34" s="4" t="s">
         <v>42</v>
       </c>
@@ -1804,7 +1814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" s="4" customFormat="1">
+    <row r="35" spans="1:10">
       <c r="A35" s="4" t="s">
         <v>42</v>
       </c>
@@ -1837,7 +1847,7 @@
         <v>0.17</v>
       </c>
     </row>
-    <row r="36" spans="1:10" s="4" customFormat="1">
+    <row r="36" spans="1:10" hidden="1">
       <c r="A36" s="4" t="s">
         <v>42</v>
       </c>
@@ -1870,7 +1880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" s="4" customFormat="1">
+    <row r="37" spans="1:10" hidden="1">
       <c r="A37" s="4" t="s">
         <v>42</v>
       </c>
@@ -1903,7 +1913,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="4" customFormat="1">
+    <row r="38" spans="1:10" hidden="1">
       <c r="A38" s="4" t="s">
         <v>42</v>
       </c>
@@ -1936,7 +1946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:10" s="4" customFormat="1">
+    <row r="39" spans="1:10" hidden="1">
       <c r="A39" s="4" t="s">
         <v>42</v>
       </c>
@@ -1969,7 +1979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:10" s="4" customFormat="1">
+    <row r="40" spans="1:10" hidden="1">
       <c r="A40" s="4" t="s">
         <v>42</v>
       </c>
@@ -2002,7 +2012,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" s="4" customFormat="1">
+    <row r="41" spans="1:10" hidden="1">
       <c r="A41" s="4" t="s">
         <v>42</v>
       </c>
@@ -2035,7 +2045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="4" customFormat="1">
+    <row r="42" spans="1:10" hidden="1">
       <c r="A42" s="4" t="s">
         <v>42</v>
       </c>
@@ -2068,7 +2078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:10" s="4" customFormat="1">
+    <row r="43" spans="1:10" hidden="1">
       <c r="A43" s="4" t="s">
         <v>42</v>
       </c>
@@ -2101,7 +2111,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" s="4" customFormat="1">
+    <row r="44" spans="1:10" hidden="1">
       <c r="A44" s="4" t="s">
         <v>42</v>
       </c>
@@ -2134,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:10" s="4" customFormat="1">
+    <row r="45" spans="1:10" hidden="1">
       <c r="A45" s="4" t="s">
         <v>42</v>
       </c>
@@ -2167,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:10" s="4" customFormat="1">
+    <row r="46" spans="1:10" hidden="1">
       <c r="A46" s="4" t="s">
         <v>42</v>
       </c>
@@ -2200,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:10" s="4" customFormat="1">
+    <row r="47" spans="1:10">
       <c r="A47" s="4" t="s">
         <v>42</v>
       </c>
@@ -2233,7 +2243,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="48" spans="1:10" s="4" customFormat="1">
+    <row r="48" spans="1:10" hidden="1">
       <c r="A48" s="4" t="s">
         <v>42</v>
       </c>
@@ -2266,7 +2276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:10" s="4" customFormat="1">
+    <row r="49" spans="1:10" hidden="1">
       <c r="A49" s="4" t="s">
         <v>42</v>
       </c>
@@ -2299,7 +2309,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:10" s="4" customFormat="1">
+    <row r="50" spans="1:10" hidden="1">
       <c r="A50" s="4" t="s">
         <v>42</v>
       </c>
@@ -2332,7 +2342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:10" s="4" customFormat="1">
+    <row r="51" spans="1:10" hidden="1">
       <c r="A51" s="4" t="s">
         <v>42</v>
       </c>
@@ -2365,7 +2375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:10" s="4" customFormat="1">
+    <row r="52" spans="1:10" hidden="1">
       <c r="A52" s="4" t="s">
         <v>42</v>
       </c>
@@ -2398,7 +2408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:10" s="4" customFormat="1">
+    <row r="53" spans="1:10">
       <c r="A53" s="4" t="s">
         <v>42</v>
       </c>
@@ -2431,7 +2441,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="54" spans="1:10" s="4" customFormat="1">
+    <row r="54" spans="1:10" hidden="1">
       <c r="A54" s="4" t="s">
         <v>42</v>
       </c>
@@ -2464,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:10" s="4" customFormat="1">
+    <row r="55" spans="1:10" hidden="1">
       <c r="A55" s="4" t="s">
         <v>42</v>
       </c>
@@ -2497,7 +2507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:10" s="4" customFormat="1">
+    <row r="56" spans="1:10" hidden="1">
       <c r="A56" s="4" t="s">
         <v>42</v>
       </c>
@@ -2530,7 +2540,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:10" s="4" customFormat="1">
+    <row r="57" spans="1:10" hidden="1">
       <c r="A57" s="4" t="s">
         <v>42</v>
       </c>
@@ -2563,7 +2573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:10" s="4" customFormat="1">
+    <row r="58" spans="1:10" hidden="1">
       <c r="A58" s="4" t="s">
         <v>42</v>
       </c>
@@ -2596,7 +2606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:10" s="4" customFormat="1">
+    <row r="59" spans="1:10" hidden="1">
       <c r="A59" s="4" t="s">
         <v>42</v>
       </c>
@@ -2629,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:10" s="4" customFormat="1">
+    <row r="60" spans="1:10">
       <c r="A60" s="4" t="s">
         <v>42</v>
       </c>
@@ -2662,7 +2672,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="61" spans="1:10" s="4" customFormat="1">
+    <row r="61" spans="1:10">
       <c r="A61" s="4" t="s">
         <v>42</v>
       </c>
@@ -2695,7 +2705,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="62" spans="1:10" s="4" customFormat="1">
+    <row r="62" spans="1:10" hidden="1">
       <c r="A62" s="4" t="s">
         <v>42</v>
       </c>
@@ -2728,7 +2738,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:10" s="4" customFormat="1">
+    <row r="63" spans="1:10" hidden="1">
       <c r="A63" s="4" t="s">
         <v>42</v>
       </c>
@@ -2761,7 +2771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:10" s="4" customFormat="1">
+    <row r="64" spans="1:10" hidden="1">
       <c r="A64" s="4" t="s">
         <v>42</v>
       </c>
@@ -2794,7 +2804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:10" s="4" customFormat="1">
+    <row r="65" spans="1:10" hidden="1">
       <c r="A65" s="4" t="s">
         <v>42</v>
       </c>
@@ -2827,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:10" s="4" customFormat="1">
+    <row r="66" spans="1:10" hidden="1">
       <c r="A66" s="4" t="s">
         <v>42</v>
       </c>
@@ -2860,7 +2870,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:10" s="4" customFormat="1">
+    <row r="67" spans="1:10" hidden="1">
       <c r="A67" s="4" t="s">
         <v>42</v>
       </c>
@@ -2893,7 +2903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:10" s="4" customFormat="1">
+    <row r="68" spans="1:10" hidden="1">
       <c r="A68" s="4" t="s">
         <v>42</v>
       </c>
@@ -2926,7 +2936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:10" s="4" customFormat="1">
+    <row r="69" spans="1:10">
       <c r="A69" s="4" t="s">
         <v>42</v>
       </c>
@@ -2959,7 +2969,7 @@
         <v>0.21</v>
       </c>
     </row>
-    <row r="70" spans="1:10" s="4" customFormat="1">
+    <row r="70" spans="1:10" hidden="1">
       <c r="A70" s="4" t="s">
         <v>42</v>
       </c>
@@ -2992,7 +3002,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:10" s="4" customFormat="1">
+    <row r="71" spans="1:10" hidden="1">
       <c r="A71" s="4" t="s">
         <v>42</v>
       </c>
@@ -3025,7 +3035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:10" s="4" customFormat="1">
+    <row r="72" spans="1:10" hidden="1">
       <c r="A72" s="4" t="s">
         <v>42</v>
       </c>
@@ -3058,7 +3068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:10" s="4" customFormat="1">
+    <row r="73" spans="1:10" hidden="1">
       <c r="A73" s="4" t="s">
         <v>42</v>
       </c>
@@ -3091,7 +3101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:10" s="4" customFormat="1">
+    <row r="74" spans="1:10" hidden="1">
       <c r="A74" s="4" t="s">
         <v>42</v>
       </c>
@@ -3124,7 +3134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:10" s="4" customFormat="1">
+    <row r="75" spans="1:10">
       <c r="A75" s="4" t="s">
         <v>42</v>
       </c>
@@ -3157,7 +3167,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="76" spans="1:10" s="4" customFormat="1">
+    <row r="76" spans="1:10" hidden="1">
       <c r="A76" s="4" t="s">
         <v>42</v>
       </c>
@@ -3190,7 +3200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:10" s="4" customFormat="1">
+    <row r="77" spans="1:10" hidden="1">
       <c r="A77" s="4" t="s">
         <v>42</v>
       </c>
@@ -3223,7 +3233,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:10" s="4" customFormat="1">
+    <row r="78" spans="1:10" hidden="1">
       <c r="A78" s="4" t="s">
         <v>42</v>
       </c>
@@ -3256,7 +3266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:10" s="4" customFormat="1">
+    <row r="79" spans="1:10" hidden="1">
       <c r="A79" s="4" t="s">
         <v>42</v>
       </c>
@@ -3289,7 +3299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:10" s="4" customFormat="1">
+    <row r="80" spans="1:10" hidden="1">
       <c r="A80" s="4" t="s">
         <v>42</v>
       </c>
@@ -3322,7 +3332,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:10" s="4" customFormat="1">
+    <row r="81" spans="1:10">
       <c r="A81" s="4" t="s">
         <v>42</v>
       </c>
@@ -3355,7 +3365,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="82" spans="1:10" s="4" customFormat="1">
+    <row r="82" spans="1:10" hidden="1">
       <c r="A82" s="4" t="s">
         <v>42</v>
       </c>
@@ -3388,7 +3398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:10" s="4" customFormat="1">
+    <row r="83" spans="1:10" hidden="1">
       <c r="A83" s="4" t="s">
         <v>42</v>
       </c>
@@ -3421,7 +3431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:10" s="4" customFormat="1">
+    <row r="84" spans="1:10" hidden="1">
       <c r="A84" s="4" t="s">
         <v>42</v>
       </c>
@@ -3454,7 +3464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:10" s="4" customFormat="1">
+    <row r="85" spans="1:10" hidden="1">
       <c r="A85" s="4" t="s">
         <v>42</v>
       </c>
@@ -3487,7 +3497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:10" s="4" customFormat="1">
+    <row r="86" spans="1:10" hidden="1">
       <c r="A86" s="4" t="s">
         <v>42</v>
       </c>
@@ -3520,7 +3530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:10" s="4" customFormat="1">
+    <row r="87" spans="1:10" hidden="1">
       <c r="A87" s="4" t="s">
         <v>42</v>
       </c>
@@ -3553,7 +3563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:10" s="4" customFormat="1">
+    <row r="88" spans="1:10">
       <c r="A88" s="4" t="s">
         <v>42</v>
       </c>
@@ -3586,7 +3596,7 @@
         <v>0.65</v>
       </c>
     </row>
-    <row r="89" spans="1:10" s="4" customFormat="1">
+    <row r="89" spans="1:10">
       <c r="A89" s="4" t="s">
         <v>42</v>
       </c>
@@ -3619,7 +3629,7 @@
         <v>0.68</v>
       </c>
     </row>
-    <row r="90" spans="1:10" s="4" customFormat="1">
+    <row r="90" spans="1:10" hidden="1">
       <c r="A90" s="4" t="s">
         <v>42</v>
       </c>
@@ -3652,7 +3662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:10" s="4" customFormat="1">
+    <row r="91" spans="1:10" hidden="1">
       <c r="A91" s="4" t="s">
         <v>42</v>
       </c>
@@ -3685,7 +3695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:10" s="4" customFormat="1">
+    <row r="92" spans="1:10" hidden="1">
       <c r="A92" s="4" t="s">
         <v>42</v>
       </c>
@@ -3718,7 +3728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:10" s="4" customFormat="1">
+    <row r="93" spans="1:10" hidden="1">
       <c r="A93" s="4" t="s">
         <v>42</v>
       </c>
@@ -3751,7 +3761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:10" s="4" customFormat="1">
+    <row r="94" spans="1:10" hidden="1">
       <c r="A94" s="4" t="s">
         <v>42</v>
       </c>
@@ -3784,7 +3794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:10" s="4" customFormat="1">
+    <row r="95" spans="1:10" hidden="1">
       <c r="A95" s="4" t="s">
         <v>42</v>
       </c>
@@ -3817,7 +3827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:10" s="4" customFormat="1">
+    <row r="96" spans="1:10">
       <c r="A96" s="4" t="s">
         <v>42</v>
       </c>
@@ -3850,7 +3860,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="97" spans="1:10" s="4" customFormat="1">
+    <row r="97" spans="1:10">
       <c r="A97" s="4" t="s">
         <v>42</v>
       </c>
@@ -3883,7 +3893,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="98" spans="1:10" s="4" customFormat="1">
+    <row r="98" spans="1:10" hidden="1">
       <c r="A98" s="4" t="s">
         <v>42</v>
       </c>
@@ -3916,7 +3926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:10" s="4" customFormat="1">
+    <row r="99" spans="1:10" hidden="1">
       <c r="A99" s="4" t="s">
         <v>42</v>
       </c>
@@ -3949,7 +3959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:10" s="4" customFormat="1">
+    <row r="100" spans="1:10">
       <c r="A100" s="4" t="s">
         <v>42</v>
       </c>
@@ -3982,7 +3992,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="101" spans="1:10" s="4" customFormat="1">
+    <row r="101" spans="1:10">
       <c r="A101" s="4" t="s">
         <v>42</v>
       </c>
@@ -4015,7 +4025,7 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="102" spans="1:10" s="4" customFormat="1">
+    <row r="102" spans="1:10" hidden="1">
       <c r="A102" s="4" t="s">
         <v>42</v>
       </c>
@@ -4048,7 +4058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:10" s="4" customFormat="1">
+    <row r="103" spans="1:10" hidden="1">
       <c r="A103" s="4" t="s">
         <v>42</v>
       </c>
@@ -4081,7 +4091,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:10" s="4" customFormat="1">
+    <row r="104" spans="1:10">
       <c r="A104" s="4" t="s">
         <v>42</v>
       </c>
@@ -4114,7 +4124,7 @@
         <v>0.77</v>
       </c>
     </row>
-    <row r="105" spans="1:10" s="4" customFormat="1">
+    <row r="105" spans="1:10">
       <c r="A105" s="4" t="s">
         <v>42</v>
       </c>
@@ -4147,7 +4157,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="106" spans="1:10" s="4" customFormat="1">
+    <row r="106" spans="1:10" hidden="1">
       <c r="A106" s="4" t="s">
         <v>42</v>
       </c>
@@ -4180,7 +4190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:10" s="4" customFormat="1">
+    <row r="107" spans="1:10" hidden="1">
       <c r="A107" s="4" t="s">
         <v>42</v>
       </c>
@@ -4213,7 +4223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:10" s="4" customFormat="1">
+    <row r="108" spans="1:10" hidden="1">
       <c r="A108" s="4" t="s">
         <v>42</v>
       </c>
@@ -4246,7 +4256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:10" s="4" customFormat="1">
+    <row r="109" spans="1:10" hidden="1">
       <c r="A109" s="4" t="s">
         <v>42</v>
       </c>
@@ -4279,7 +4289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:10" s="4" customFormat="1">
+    <row r="110" spans="1:10" hidden="1">
       <c r="A110" s="4" t="s">
         <v>42</v>
       </c>
@@ -4312,7 +4322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:10" s="4" customFormat="1">
+    <row r="111" spans="1:10" hidden="1">
       <c r="A111" s="4" t="s">
         <v>42</v>
       </c>
@@ -4345,7 +4355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:10" s="4" customFormat="1">
+    <row r="112" spans="1:10">
       <c r="A112" s="4" t="s">
         <v>42</v>
       </c>
@@ -4378,7 +4388,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="113" spans="1:10" s="4" customFormat="1">
+    <row r="113" spans="1:10">
       <c r="A113" s="4" t="s">
         <v>42</v>
       </c>
@@ -4411,7 +4421,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="114" spans="1:10" s="4" customFormat="1">
+    <row r="114" spans="1:10" hidden="1">
       <c r="A114" s="4" t="s">
         <v>42</v>
       </c>
@@ -4444,7 +4454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:10" s="4" customFormat="1">
+    <row r="115" spans="1:10" hidden="1">
       <c r="A115" s="4" t="s">
         <v>42</v>
       </c>
@@ -4477,7 +4487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:10" s="4" customFormat="1">
+    <row r="116" spans="1:10" hidden="1">
       <c r="A116" s="4" t="s">
         <v>42</v>
       </c>
@@ -4510,7 +4520,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:10" s="4" customFormat="1">
+    <row r="117" spans="1:10" hidden="1">
       <c r="A117" s="4" t="s">
         <v>42</v>
       </c>
@@ -4543,7 +4553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:10" s="4" customFormat="1">
+    <row r="118" spans="1:10" hidden="1">
       <c r="A118" s="4" t="s">
         <v>42</v>
       </c>
@@ -4576,7 +4586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:10" s="4" customFormat="1">
+    <row r="119" spans="1:10" hidden="1">
       <c r="A119" s="4" t="s">
         <v>42</v>
       </c>
@@ -4609,7 +4619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:10" s="4" customFormat="1">
+    <row r="120" spans="1:10">
       <c r="A120" s="4" t="s">
         <v>42</v>
       </c>
@@ -4642,7 +4652,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="121" spans="1:10" s="4" customFormat="1">
+    <row r="121" spans="1:10">
       <c r="A121" s="4" t="s">
         <v>42</v>
       </c>
@@ -4675,7 +4685,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="122" spans="1:10" s="4" customFormat="1">
+    <row r="122" spans="1:10" hidden="1">
       <c r="A122" s="4" t="s">
         <v>42</v>
       </c>
@@ -4708,7 +4718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:10" s="4" customFormat="1">
+    <row r="123" spans="1:10" hidden="1">
       <c r="A123" s="4" t="s">
         <v>42</v>
       </c>
@@ -4741,7 +4751,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:10" s="4" customFormat="1">
+    <row r="124" spans="1:10" hidden="1">
       <c r="A124" s="4" t="s">
         <v>42</v>
       </c>
@@ -4774,7 +4784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:10" s="4" customFormat="1">
+    <row r="125" spans="1:10" hidden="1">
       <c r="A125" s="4" t="s">
         <v>42</v>
       </c>
@@ -4807,7 +4817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:10" s="4" customFormat="1">
+    <row r="126" spans="1:10" hidden="1">
       <c r="A126" s="4" t="s">
         <v>42</v>
       </c>
@@ -4840,7 +4850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:10" s="4" customFormat="1">
+    <row r="127" spans="1:10" hidden="1">
       <c r="A127" s="4" t="s">
         <v>42</v>
       </c>
@@ -4873,7 +4883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:10" s="4" customFormat="1">
+    <row r="128" spans="1:10">
       <c r="A128" s="4" t="s">
         <v>42</v>
       </c>
@@ -4906,7 +4916,7 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="129" spans="1:10" s="4" customFormat="1">
+    <row r="129" spans="1:10">
       <c r="A129" s="4" t="s">
         <v>42</v>
       </c>
@@ -4940,6 +4950,30 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K129">
+    <filterColumn colId="9">
+      <filters>
+        <filter val="0.05"/>
+        <filter val="0.11"/>
+        <filter val="0.12"/>
+        <filter val="0.17"/>
+        <filter val="0.18"/>
+        <filter val="0.20"/>
+        <filter val="0.21"/>
+        <filter val="0.27"/>
+        <filter val="0.28"/>
+        <filter val="0.30"/>
+        <filter val="0.42"/>
+        <filter val="0.60"/>
+        <filter val="0.61"/>
+        <filter val="0.65"/>
+        <filter val="0.68"/>
+        <filter val="0.70"/>
+        <filter val="0.77"/>
+        <filter val="0.93"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>

</xml_diff>